<commit_message>
update jags to reflect subadults in pen
</commit_message>
<xml_diff>
--- a/data/KZ/Count_summary_KZ.xlsx
+++ b/data/KZ/Count_summary_KZ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clayton.lamb/Google Drive/Documents/University/PDF/analyses/KZdemography/KZ_QT_IPM/data/KZ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8D7E0F-9426-6847-81DF-EA818A0A6597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B3C331-3050-0C4E-8429-C32D67F48B5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31620" yWindow="460" windowWidth="31000" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="1500" windowWidth="31000" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MinCount_summary_KZ-withimm" sheetId="2" r:id="rId1"/>
@@ -1008,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
2021 update, first commit
</commit_message>
<xml_diff>
--- a/data/KZ/Count_summary_KZ.xlsx
+++ b/data/KZ/Count_summary_KZ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clayton.lamb/Google Drive/Documents/University/PDF/analyses/KZdemography/KZ_QT_IPM/data/KZ/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clayton.lamb/Google Drive/Documents/University/PDF/PDF Analyses/KZdemography/KZ_QT_IPM/data/KZ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B3C331-3050-0C4E-8429-C32D67F48B5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11764697-2ADF-3144-B6CA-70BA37DCBA65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="1500" windowWidth="31000" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32400" yWindow="1440" windowWidth="31000" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MinCount_summary_KZ-withimm" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>Year</t>
   </si>
@@ -1006,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Y27"/>
+  <dimension ref="A1:Y28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1682,11 +1682,11 @@
         <v>0.64</v>
       </c>
       <c r="O19">
-        <f t="shared" ref="O19:O27" si="6">AVERAGE(J19:K19)</f>
+        <f t="shared" ref="O19:O28" si="6">AVERAGE(J19:K19)</f>
         <v>37.799999999999997</v>
       </c>
       <c r="P19">
-        <f t="shared" ref="P19:P27" si="7">AVERAGE(H19:I19)</f>
+        <f t="shared" ref="P19:P28" si="7">AVERAGE(H19:I19)</f>
         <v>7.2000000000000011</v>
       </c>
       <c r="Q19">
@@ -1828,11 +1828,11 @@
         <v>6</v>
       </c>
       <c r="J21">
-        <f t="shared" ref="J21:J27" si="8">E21-H21</f>
+        <f t="shared" ref="J21:J28" si="8">E21-H21</f>
         <v>34</v>
       </c>
       <c r="K21">
-        <f t="shared" ref="K21:K27" si="9">F21-I21</f>
+        <f t="shared" ref="K21:K28" si="9">F21-I21</f>
         <v>34</v>
       </c>
       <c r="L21">
@@ -1893,7 +1893,7 @@
         <v>6</v>
       </c>
       <c r="H22">
-        <f t="shared" ref="H22:I27" si="10">G22</f>
+        <f t="shared" ref="H22:I28" si="10">G22</f>
         <v>6</v>
       </c>
       <c r="I22">
@@ -1933,19 +1933,19 @@
         <v>0.09</v>
       </c>
       <c r="S22">
-        <f t="shared" ref="S22:S27" si="11">AVERAGE(J22:K22)/Q22</f>
+        <f t="shared" ref="S22:S28" si="11">AVERAGE(J22:K22)/Q22</f>
         <v>36</v>
       </c>
       <c r="T22">
-        <f t="shared" ref="T22:T27" si="12">AVERAGE(J22:K22)*R22</f>
+        <f t="shared" ref="T22:T28" si="12">AVERAGE(J22:K22)*R22</f>
         <v>3.2399999999999998</v>
       </c>
       <c r="U22">
-        <f t="shared" ref="U22:U27" si="13">AVERAGE(H22:I22)/Q22</f>
+        <f t="shared" ref="U22:U28" si="13">AVERAGE(H22:I22)/Q22</f>
         <v>6</v>
       </c>
       <c r="V22">
-        <f t="shared" ref="V22:V27" si="14">AVERAGE(H22:I22)*R22</f>
+        <f t="shared" ref="V22:V28" si="14">AVERAGE(H22:I22)*R22</f>
         <v>0.54</v>
       </c>
       <c r="W22" t="s">
@@ -2314,6 +2314,79 @@
         <v>1.26</v>
       </c>
       <c r="W27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2021</v>
+      </c>
+      <c r="E28">
+        <v>101</v>
+      </c>
+      <c r="F28">
+        <v>101</v>
+      </c>
+      <c r="G28" s="1">
+        <v>14</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="10"/>
+        <v>14</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="10"/>
+        <v>14</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="8"/>
+        <v>87</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="9"/>
+        <v>87</v>
+      </c>
+      <c r="L28">
+        <v>37</v>
+      </c>
+      <c r="M28">
+        <v>37</v>
+      </c>
+      <c r="N28">
+        <f>M28/K28</f>
+        <v>0.42528735632183906</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="6"/>
+        <v>87</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <v>0.09</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="11"/>
+        <v>87</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="12"/>
+        <v>7.83</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
+      <c r="V28">
+        <f t="shared" si="14"/>
+        <v>1.26</v>
+      </c>
+      <c r="W28" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update meanr and means tau to 0.01, from 100, as per reviewer comments
</commit_message>
<xml_diff>
--- a/data/KZ/Count_summary_KZ.xlsx
+++ b/data/KZ/Count_summary_KZ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clayton.lamb/Google Drive/Documents/University/PDF/PDF Analyses/KZdemography/KZ_QT_IPM/data/KZ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553D2C23-B7FC-7541-AC4A-DCD19D553982}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971047DB-54F1-F241-8BD2-BB4BA9566A0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38720" yWindow="500" windowWidth="38400" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MinCount_summary_KZ-withimm" sheetId="2" r:id="rId1"/>
@@ -1008,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W34" sqref="W34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1287,41 +1287,65 @@
       <c r="A4">
         <v>1997</v>
       </c>
+      <c r="N4">
+        <v>0.64</v>
+      </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1998</v>
       </c>
+      <c r="N5">
+        <v>0.64</v>
+      </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1999</v>
       </c>
+      <c r="N6">
+        <v>0.64</v>
+      </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2000</v>
       </c>
+      <c r="N7">
+        <v>0.64</v>
+      </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2001</v>
       </c>
+      <c r="N8">
+        <v>0.64</v>
+      </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2002</v>
       </c>
+      <c r="N9">
+        <v>0.64</v>
+      </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2003</v>
       </c>
+      <c r="N10">
+        <v>0.64</v>
+      </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2004</v>
       </c>
+      <c r="N11">
+        <v>0.64</v>
+      </c>
       <c r="X11" t="s">
         <v>29</v>
       </c>
@@ -1381,7 +1405,6 @@
         <v>30.271999999999998</v>
       </c>
       <c r="N12">
-        <f>M12/K12</f>
         <v>0.64</v>
       </c>
       <c r="O12">
@@ -1422,16 +1445,25 @@
       <c r="A13">
         <v>2006</v>
       </c>
+      <c r="N13">
+        <v>0.64</v>
+      </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2007</v>
       </c>
+      <c r="N14">
+        <v>0.64</v>
+      </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2008</v>
       </c>
+      <c r="N15">
+        <v>0.64</v>
+      </c>
       <c r="X15" s="2" t="s">
         <v>30</v>
       </c>
@@ -1491,8 +1523,7 @@
         <v>32.870400000000004</v>
       </c>
       <c r="N16">
-        <f t="shared" si="1"/>
-        <v>0.64000000000000012</v>
+        <v>0.64</v>
       </c>
       <c r="O16">
         <f>AVERAGE(J16:K16)</f>
@@ -1531,6 +1562,9 @@
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2010</v>
+      </c>
+      <c r="N17">
+        <v>0.64</v>
       </c>
       <c r="X17" s="2" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
tidy data, update results
</commit_message>
<xml_diff>
--- a/data/KZ/Count_summary_KZ.xlsx
+++ b/data/KZ/Count_summary_KZ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clayton.lamb/Google Drive/Documents/University/PDF/PDF Analyses/KZdemography/KZ_QT_IPM/data/KZ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971047DB-54F1-F241-8BD2-BB4BA9566A0A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAA676D-8487-8642-82E2-058B49434311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38720" yWindow="500" windowWidth="38400" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MinCount_summary_KZ-withimm" sheetId="2" r:id="rId1"/>
@@ -1008,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q34" sqref="Q34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V35" sqref="V35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1240,7 +1240,7 @@
         <v>125.34399999999999</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N26" si="1">M3/K3</f>
+        <f t="shared" ref="N3:N20" si="1">M3/K3</f>
         <v>0.64</v>
       </c>
       <c r="O3">
@@ -1346,12 +1346,6 @@
       <c r="N11">
         <v>0.64</v>
       </c>
-      <c r="X11" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y11" s="2" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -1440,6 +1434,12 @@
       <c r="W12" t="s">
         <v>21</v>
       </c>
+      <c r="X12" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1464,12 +1464,6 @@
       <c r="N15">
         <v>0.64</v>
       </c>
-      <c r="X15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y15" s="2" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -1558,6 +1552,12 @@
       <c r="W16" t="s">
         <v>28</v>
       </c>
+      <c r="X16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y16" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -1566,9 +1566,6 @@
       <c r="N17">
         <v>0.64</v>
       </c>
-      <c r="X17" s="2" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -1658,7 +1655,7 @@
         <v>32</v>
       </c>
       <c r="X18" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
@@ -1749,7 +1746,7 @@
         <v>27</v>
       </c>
       <c r="X19" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.2">
@@ -1839,6 +1836,9 @@
       <c r="W20" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="X20" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21">
@@ -1876,11 +1876,11 @@
         <v>22</v>
       </c>
       <c r="N21">
-        <f>M21/K21</f>
+        <f>AVERAGE(L21:M21)/AVERAGE(J21:K21)</f>
         <v>0.6875</v>
       </c>
       <c r="O21">
-        <f t="shared" si="6"/>
+        <f>AVERAGE(J21:K21)</f>
         <v>32</v>
       </c>
       <c r="P21">
@@ -1949,8 +1949,8 @@
         <v>27</v>
       </c>
       <c r="N22">
-        <f t="shared" si="1"/>
-        <v>0.77142857142857146</v>
+        <f t="shared" ref="N22:N28" si="11">AVERAGE(L22:M22)/AVERAGE(J22:K22)</f>
+        <v>0.74285714285714288</v>
       </c>
       <c r="O22">
         <f t="shared" si="6"/>
@@ -1967,19 +1967,19 @@
         <v>0.09</v>
       </c>
       <c r="S22">
-        <f t="shared" ref="S22:S28" si="11">AVERAGE(J22:K22)/Q22</f>
+        <f t="shared" ref="S22:S28" si="12">AVERAGE(J22:K22)/Q22</f>
         <v>35</v>
       </c>
       <c r="T22">
-        <f t="shared" ref="T22:T28" si="12">AVERAGE(J22:K22)*R22</f>
+        <f t="shared" ref="T22:T28" si="13">AVERAGE(J22:K22)*R22</f>
         <v>3.15</v>
       </c>
       <c r="U22">
-        <f t="shared" ref="U22:U28" si="13">AVERAGE(H22:I22)/Q22</f>
+        <f t="shared" ref="U22:U28" si="14">AVERAGE(H22:I22)/Q22</f>
         <v>6</v>
       </c>
       <c r="V22">
-        <f t="shared" ref="V22:V28" si="14">AVERAGE(H22:I22)*R22</f>
+        <f t="shared" ref="V22:V28" si="15">AVERAGE(H22:I22)*R22</f>
         <v>0.54</v>
       </c>
       <c r="W22" t="s">
@@ -2022,8 +2022,8 @@
         <v>30</v>
       </c>
       <c r="N23">
-        <f t="shared" si="1"/>
-        <v>0.66666666666666663</v>
+        <f t="shared" si="11"/>
+        <v>0.65555555555555556</v>
       </c>
       <c r="O23">
         <f t="shared" si="6"/>
@@ -2040,19 +2040,19 @@
         <v>0.09</v>
       </c>
       <c r="S23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>45</v>
       </c>
       <c r="T23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.05</v>
       </c>
       <c r="U23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>9</v>
       </c>
       <c r="V23">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.80999999999999994</v>
       </c>
       <c r="W23" t="s">
@@ -2095,8 +2095,8 @@
         <v>25</v>
       </c>
       <c r="N24">
-        <f t="shared" si="1"/>
-        <v>0.52083333333333337</v>
+        <f t="shared" si="11"/>
+        <v>0.58333333333333337</v>
       </c>
       <c r="O24">
         <f t="shared" si="6"/>
@@ -2113,19 +2113,19 @@
         <v>0.09</v>
       </c>
       <c r="S24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>48</v>
       </c>
       <c r="T24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.32</v>
       </c>
       <c r="U24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>12</v>
       </c>
       <c r="V24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.08</v>
       </c>
       <c r="W24" t="s">
@@ -2166,8 +2166,8 @@
         <v>34</v>
       </c>
       <c r="N25">
-        <f t="shared" si="1"/>
-        <v>0.64150943396226412</v>
+        <f t="shared" si="11"/>
+        <v>0.57547169811320753</v>
       </c>
       <c r="O25">
         <f t="shared" si="6"/>
@@ -2184,19 +2184,19 @@
         <v>0.09</v>
       </c>
       <c r="S25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>53</v>
       </c>
       <c r="T25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.7699999999999996</v>
       </c>
       <c r="U25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>13</v>
       </c>
       <c r="V25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.17</v>
       </c>
       <c r="W25" t="s">
@@ -2239,8 +2239,8 @@
         <v>33</v>
       </c>
       <c r="N26">
-        <f t="shared" si="1"/>
-        <v>0.47142857142857142</v>
+        <f t="shared" si="11"/>
+        <v>0.51428571428571423</v>
       </c>
       <c r="O26">
         <f t="shared" si="6"/>
@@ -2257,19 +2257,19 @@
         <v>0.27</v>
       </c>
       <c r="S26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>70</v>
       </c>
       <c r="T26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>18.900000000000002</v>
       </c>
       <c r="U26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>11</v>
       </c>
       <c r="V26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>2.97</v>
       </c>
       <c r="W26" t="s">
@@ -2312,8 +2312,8 @@
         <v>29</v>
       </c>
       <c r="N27">
-        <f>M27/K27</f>
-        <v>0.41428571428571431</v>
+        <f t="shared" si="11"/>
+        <v>0.42142857142857143</v>
       </c>
       <c r="O27">
         <f t="shared" si="6"/>
@@ -2330,19 +2330,19 @@
         <v>0.09</v>
       </c>
       <c r="S27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>70</v>
       </c>
       <c r="T27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6.3</v>
       </c>
       <c r="U27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="V27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.26</v>
       </c>
       <c r="W27" t="s">
@@ -2385,8 +2385,8 @@
         <v>37</v>
       </c>
       <c r="N28">
-        <f>M28/K28</f>
-        <v>0.42528735632183906</v>
+        <f t="shared" si="11"/>
+        <v>0.43103448275862066</v>
       </c>
       <c r="O28">
         <f t="shared" si="6"/>
@@ -2403,19 +2403,19 @@
         <v>0.09</v>
       </c>
       <c r="S28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>87</v>
       </c>
       <c r="T28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>7.83</v>
       </c>
       <c r="U28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="V28">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.26</v>
       </c>
       <c r="W28" t="s">

</xml_diff>

<commit_message>
update survival and count errors
</commit_message>
<xml_diff>
--- a/data/KZ/Count_summary_KZ.xlsx
+++ b/data/KZ/Count_summary_KZ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clayton.lamb/Google Drive/Documents/University/PDF/PDF Analyses/KZdemography/KZ_QT_IPM/data/KZ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAA676D-8487-8642-82E2-058B49434311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C217CC4-6BE4-AF44-AB75-853FC66C5F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1008,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V35" sqref="V35"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1164,23 +1164,23 @@
         <v>0.7</v>
       </c>
       <c r="R2">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="S2">
         <f>AVERAGE(J2:K2)/Q2</f>
         <v>279.00000000000006</v>
       </c>
       <c r="T2">
-        <f>AVERAGE(J2:K2)*R2</f>
-        <v>58.59</v>
+        <f>(AVERAGE(J2:K2)/(Q2-R2))-S2</f>
+        <v>111.60000000000002</v>
       </c>
       <c r="U2">
         <f>AVERAGE(H2:I2)/Q2</f>
         <v>31.000000000000007</v>
       </c>
       <c r="V2">
-        <f>AVERAGE(H2:I2)*R2</f>
-        <v>6.5100000000000007</v>
+        <f>(AVERAGE(H2:I2)/(Q2-R2))-U2</f>
+        <v>12.400000000000006</v>
       </c>
       <c r="W2" t="s">
         <v>18</v>
@@ -1255,23 +1255,23 @@
         <v>0.7</v>
       </c>
       <c r="R3">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="S3">
         <f>AVERAGE(J3:K3)/Q3</f>
         <v>270.68571428571431</v>
       </c>
       <c r="T3">
-        <f>AVERAGE(J3:K3)*R3</f>
-        <v>56.844000000000001</v>
+        <f>(AVERAGE(J3:K3)/(Q3-R3))-S3</f>
+        <v>108.27428571428578</v>
       </c>
       <c r="U3">
         <f>AVERAGE(H3:I3)/Q3</f>
         <v>27.885714285714286</v>
       </c>
       <c r="V3">
-        <f>AVERAGE(H3:I3)*R3</f>
-        <v>5.8559999999999999</v>
+        <f>(AVERAGE(H3:I3)/(Q3-R3))-U3</f>
+        <v>11.15428571428572</v>
       </c>
       <c r="W3" t="s">
         <v>18</v>
@@ -1420,16 +1420,16 @@
         <v>67.571428571428569</v>
       </c>
       <c r="T12">
-        <f>AVERAGE(J12:K12)*R12</f>
-        <v>11.824999999999999</v>
+        <f>(AVERAGE(J12:K12)/(Q12-R12))-S12</f>
+        <v>37.539682539682545</v>
       </c>
       <c r="U12">
         <f>AVERAGE(H12:I12)/Q12</f>
         <v>11.000000000000002</v>
       </c>
       <c r="V12">
-        <f>AVERAGE(H12:I12)*R12</f>
-        <v>1.925</v>
+        <f>(AVERAGE(H12:I12)/(Q12-R12))-U12</f>
+        <v>6.1111111111111125</v>
       </c>
       <c r="W12" t="s">
         <v>21</v>
@@ -1538,16 +1538,16 @@
         <v>74.771428571428586</v>
       </c>
       <c r="T16">
-        <f>AVERAGE(J16:K16)*R16</f>
-        <v>13.085000000000001</v>
+        <f>(AVERAGE(J16:K16)/(Q16-R16))-S16</f>
+        <v>41.539682539682545</v>
       </c>
       <c r="U16">
         <f>AVERAGE(H16:I16)/Q16</f>
         <v>13.800000000000004</v>
       </c>
       <c r="V16">
-        <f>AVERAGE(H16:I16)*R16</f>
-        <v>2.4150000000000005</v>
+        <f>(AVERAGE(H16:I16)/(Q16-R16))-U16</f>
+        <v>7.6666666666666679</v>
       </c>
       <c r="W16" t="s">
         <v>28</v>
@@ -1640,16 +1640,16 @@
         <v>48.8</v>
       </c>
       <c r="T18">
-        <f>AVERAGE(J18:K18)*R18</f>
-        <v>5.8559999999999999</v>
+        <f>(AVERAGE(J18:K18)/(Q18-R18))-S18</f>
+        <v>6.6545454545454561</v>
       </c>
       <c r="U18">
         <f>AVERAGE(H18:I18)/Q18</f>
         <v>6.2000000000000011</v>
       </c>
       <c r="V18">
-        <f>AVERAGE(H18:I18)*R18</f>
-        <v>0.74400000000000011</v>
+        <f>(AVERAGE(H18:I18)/(Q18-R18))-U18</f>
+        <v>0.84545454545454568</v>
       </c>
       <c r="W18" t="s">
         <v>32</v>
@@ -1724,23 +1724,23 @@
         <v>1</v>
       </c>
       <c r="R19">
-        <v>0.2</v>
+        <v>0.09</v>
       </c>
       <c r="S19">
         <f>AVERAGE(J19:K19)/Q19</f>
         <v>37.799999999999997</v>
       </c>
       <c r="T19">
-        <f>AVERAGE(J19:K19)*R19</f>
-        <v>7.56</v>
+        <f>(AVERAGE(J19:K19)/(Q19-R19))-S19</f>
+        <v>3.7384615384615358</v>
       </c>
       <c r="U19">
         <f>AVERAGE(H19:I19)/Q19</f>
         <v>7.2000000000000011</v>
       </c>
       <c r="V19">
-        <f>AVERAGE(H19:I19)*R19</f>
-        <v>1.4400000000000004</v>
+        <f t="shared" ref="V19:V28" si="8">(AVERAGE(H19:I19)/(Q19-R19))-U19</f>
+        <v>0.71208791208791222</v>
       </c>
       <c r="W19" s="2" t="s">
         <v>27</v>
@@ -1822,16 +1822,16 @@
         <v>30.8</v>
       </c>
       <c r="T20">
-        <f>AVERAGE(J20:K20)*R20</f>
-        <v>2.7719999999999998</v>
+        <f>(AVERAGE(J20:K20)/(Q20-R20))-S20</f>
+        <v>3.046153846153846</v>
       </c>
       <c r="U20">
         <f>AVERAGE(H20:I20)/Q20</f>
         <v>5.2</v>
       </c>
       <c r="V20">
-        <f>AVERAGE(H20:I20)*R20</f>
-        <v>0.46799999999999997</v>
+        <f t="shared" si="8"/>
+        <v>0.51428571428571423</v>
       </c>
       <c r="W20" s="2" t="s">
         <v>34</v>
@@ -1898,16 +1898,16 @@
         <v>32</v>
       </c>
       <c r="T21">
-        <f>AVERAGE(J21:K21)*R21</f>
-        <v>2.88</v>
+        <f>(AVERAGE(J21:K21)/(Q21-R21))-S21</f>
+        <v>3.1648351648351607</v>
       </c>
       <c r="U21">
         <f>AVERAGE(H21:I21)/Q21</f>
         <v>6</v>
       </c>
       <c r="V21">
-        <f>AVERAGE(H21:I21)*R21</f>
-        <v>0.54</v>
+        <f t="shared" si="8"/>
+        <v>0.59340659340659307</v>
       </c>
       <c r="W21" t="s">
         <v>36</v>
@@ -1918,22 +1918,22 @@
         <v>2015</v>
       </c>
       <c r="E22">
-        <f t="shared" ref="E22:E28" si="8">J22+H22</f>
+        <f t="shared" ref="E22:E28" si="9">J22+H22</f>
         <v>41</v>
       </c>
       <c r="F22">
-        <f t="shared" ref="F22:F28" si="9">K22+I22</f>
+        <f t="shared" ref="F22:F28" si="10">K22+I22</f>
         <v>41</v>
       </c>
       <c r="G22" s="1">
         <v>6</v>
       </c>
       <c r="H22">
-        <f t="shared" ref="H22:I28" si="10">G22</f>
+        <f t="shared" ref="H22:I28" si="11">G22</f>
         <v>6</v>
       </c>
       <c r="I22">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6</v>
       </c>
       <c r="J22">
@@ -1949,7 +1949,7 @@
         <v>27</v>
       </c>
       <c r="N22">
-        <f t="shared" ref="N22:N28" si="11">AVERAGE(L22:M22)/AVERAGE(J22:K22)</f>
+        <f>AVERAGE(L22:M22)/AVERAGE(J22:K22)</f>
         <v>0.74285714285714288</v>
       </c>
       <c r="O22">
@@ -1971,16 +1971,16 @@
         <v>35</v>
       </c>
       <c r="T22">
-        <f t="shared" ref="T22:T28" si="13">AVERAGE(J22:K22)*R22</f>
-        <v>3.15</v>
+        <f>(AVERAGE(J22:K22)/(Q22-R22))-S22</f>
+        <v>3.4615384615384599</v>
       </c>
       <c r="U22">
-        <f t="shared" ref="U22:U28" si="14">AVERAGE(H22:I22)/Q22</f>
+        <f t="shared" ref="U22:U28" si="13">AVERAGE(H22:I22)/Q22</f>
         <v>6</v>
       </c>
       <c r="V22">
-        <f t="shared" ref="V22:V28" si="15">AVERAGE(H22:I22)*R22</f>
-        <v>0.54</v>
+        <f t="shared" si="8"/>
+        <v>0.59340659340659307</v>
       </c>
       <c r="W22" t="s">
         <v>36</v>
@@ -1991,22 +1991,22 @@
         <v>2016</v>
       </c>
       <c r="E23">
-        <f t="shared" si="8"/>
-        <v>54</v>
-      </c>
-      <c r="F23">
         <f t="shared" si="9"/>
         <v>54</v>
       </c>
+      <c r="F23">
+        <f t="shared" si="10"/>
+        <v>54</v>
+      </c>
       <c r="G23" s="1">
         <v>9</v>
       </c>
       <c r="H23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="I23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9</v>
       </c>
       <c r="J23">
@@ -2022,7 +2022,7 @@
         <v>30</v>
       </c>
       <c r="N23">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="N23:N28" si="14">AVERAGE(L23:M23)/AVERAGE(J23:K23)</f>
         <v>0.65555555555555556</v>
       </c>
       <c r="O23">
@@ -2044,16 +2044,16 @@
         <v>45</v>
       </c>
       <c r="T23">
+        <f>(AVERAGE(J23:K23)/(Q23-R23))-S23</f>
+        <v>4.4505494505494454</v>
+      </c>
+      <c r="U23">
         <f t="shared" si="13"/>
-        <v>4.05</v>
-      </c>
-      <c r="U23">
-        <f t="shared" si="14"/>
         <v>9</v>
       </c>
       <c r="V23">
-        <f t="shared" si="15"/>
-        <v>0.80999999999999994</v>
+        <f t="shared" si="8"/>
+        <v>0.8901098901098905</v>
       </c>
       <c r="W23" t="s">
         <v>36</v>
@@ -2064,22 +2064,22 @@
         <v>2017</v>
       </c>
       <c r="E24">
-        <f t="shared" si="8"/>
-        <v>60</v>
-      </c>
-      <c r="F24">
         <f t="shared" si="9"/>
         <v>60</v>
       </c>
+      <c r="F24">
+        <f t="shared" si="10"/>
+        <v>60</v>
+      </c>
       <c r="G24" s="1">
         <v>12</v>
       </c>
       <c r="H24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
       <c r="I24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>12</v>
       </c>
       <c r="J24">
@@ -2095,7 +2095,7 @@
         <v>25</v>
       </c>
       <c r="N24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.58333333333333337</v>
       </c>
       <c r="O24">
@@ -2117,16 +2117,16 @@
         <v>48</v>
       </c>
       <c r="T24">
+        <f>(AVERAGE(J24:K24)/(Q24-R24))-S24</f>
+        <v>4.7472527472527446</v>
+      </c>
+      <c r="U24">
         <f t="shared" si="13"/>
-        <v>4.32</v>
-      </c>
-      <c r="U24">
-        <f t="shared" si="14"/>
         <v>12</v>
       </c>
       <c r="V24">
-        <f t="shared" si="15"/>
-        <v>1.08</v>
+        <f t="shared" si="8"/>
+        <v>1.1868131868131861</v>
       </c>
       <c r="W24" t="s">
         <v>36</v>
@@ -2137,13 +2137,13 @@
         <v>2018</v>
       </c>
       <c r="E25">
-        <f t="shared" si="8"/>
-        <v>66</v>
-      </c>
-      <c r="F25">
         <f t="shared" si="9"/>
         <v>66</v>
       </c>
+      <c r="F25">
+        <f t="shared" si="10"/>
+        <v>66</v>
+      </c>
       <c r="G25" s="1">
         <v>12</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>34</v>
       </c>
       <c r="N25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.57547169811320753</v>
       </c>
       <c r="O25">
@@ -2188,16 +2188,16 @@
         <v>53</v>
       </c>
       <c r="T25">
+        <f>(AVERAGE(J25:K25)/(Q25-R25))-S25</f>
+        <v>5.2417582417582409</v>
+      </c>
+      <c r="U25">
         <f t="shared" si="13"/>
-        <v>4.7699999999999996</v>
-      </c>
-      <c r="U25">
-        <f t="shared" si="14"/>
         <v>13</v>
       </c>
       <c r="V25">
-        <f t="shared" si="15"/>
-        <v>1.17</v>
+        <f t="shared" si="8"/>
+        <v>1.2857142857142847</v>
       </c>
       <c r="W25" t="s">
         <v>36</v>
@@ -2208,22 +2208,22 @@
         <v>2019</v>
       </c>
       <c r="E26">
-        <f t="shared" si="8"/>
-        <v>81</v>
-      </c>
-      <c r="F26">
         <f t="shared" si="9"/>
         <v>81</v>
       </c>
+      <c r="F26">
+        <f t="shared" si="10"/>
+        <v>81</v>
+      </c>
       <c r="G26" s="1">
         <v>11</v>
       </c>
       <c r="H26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
       <c r="I26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
       <c r="J26">
@@ -2239,7 +2239,7 @@
         <v>33</v>
       </c>
       <c r="N26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.51428571428571423</v>
       </c>
       <c r="O26">
@@ -2254,23 +2254,23 @@
         <v>1</v>
       </c>
       <c r="R26">
-        <v>0.27</v>
+        <v>0.09</v>
       </c>
       <c r="S26">
         <f t="shared" si="12"/>
         <v>70</v>
       </c>
       <c r="T26">
+        <f>(AVERAGE(J26:K26)/(Q26-R26))-S26</f>
+        <v>6.9230769230769198</v>
+      </c>
+      <c r="U26">
         <f t="shared" si="13"/>
-        <v>18.900000000000002</v>
-      </c>
-      <c r="U26">
-        <f t="shared" si="14"/>
         <v>11</v>
       </c>
       <c r="V26">
-        <f t="shared" si="15"/>
-        <v>2.97</v>
+        <f t="shared" si="8"/>
+        <v>1.0879120879120876</v>
       </c>
       <c r="W26" t="s">
         <v>36</v>
@@ -2281,22 +2281,22 @@
         <v>2020</v>
       </c>
       <c r="E27">
-        <f t="shared" si="8"/>
-        <v>84</v>
-      </c>
-      <c r="F27">
         <f t="shared" si="9"/>
         <v>84</v>
       </c>
+      <c r="F27">
+        <f t="shared" si="10"/>
+        <v>84</v>
+      </c>
       <c r="G27" s="1">
         <v>14</v>
       </c>
       <c r="H27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>14</v>
       </c>
       <c r="I27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>14</v>
       </c>
       <c r="J27">
@@ -2312,7 +2312,7 @@
         <v>29</v>
       </c>
       <c r="N27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.42142857142857143</v>
       </c>
       <c r="O27">
@@ -2334,16 +2334,16 @@
         <v>70</v>
       </c>
       <c r="T27">
+        <f>(AVERAGE(J27:K27)/(Q27-R27))-S27</f>
+        <v>6.9230769230769198</v>
+      </c>
+      <c r="U27">
         <f t="shared" si="13"/>
-        <v>6.3</v>
-      </c>
-      <c r="U27">
-        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="V27">
-        <f t="shared" si="15"/>
-        <v>1.26</v>
+        <f t="shared" si="8"/>
+        <v>1.3846153846153832</v>
       </c>
       <c r="W27" t="s">
         <v>36</v>
@@ -2354,22 +2354,22 @@
         <v>2021</v>
       </c>
       <c r="E28">
-        <f t="shared" si="8"/>
-        <v>101</v>
-      </c>
-      <c r="F28">
         <f t="shared" si="9"/>
         <v>101</v>
       </c>
+      <c r="F28">
+        <f t="shared" si="10"/>
+        <v>101</v>
+      </c>
       <c r="G28" s="1">
         <v>14</v>
       </c>
       <c r="H28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>14</v>
       </c>
       <c r="I28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>14</v>
       </c>
       <c r="J28">
@@ -2385,7 +2385,7 @@
         <v>37</v>
       </c>
       <c r="N28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.43103448275862066</v>
       </c>
       <c r="O28">
@@ -2407,16 +2407,16 @@
         <v>87</v>
       </c>
       <c r="T28">
+        <f>(AVERAGE(J28:K28)/(Q28-R28))-S28</f>
+        <v>8.6043956043956058</v>
+      </c>
+      <c r="U28">
         <f t="shared" si="13"/>
-        <v>7.83</v>
-      </c>
-      <c r="U28">
-        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="V28">
-        <f t="shared" si="15"/>
-        <v>1.26</v>
+        <f t="shared" si="8"/>
+        <v>1.3846153846153832</v>
       </c>
       <c r="W28" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
add erorr bars to observed rates in plots
</commit_message>
<xml_diff>
--- a/data/KZ/Count_summary_KZ.xlsx
+++ b/data/KZ/Count_summary_KZ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clayton.lamb/Google Drive/Documents/University/PDF/PDF Analyses/KZdemography/KZ_QT_IPM/data/KZ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C217CC4-6BE4-AF44-AB75-853FC66C5F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A33053-75A3-834C-92C5-258BC28A478F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40800" yWindow="500" windowWidth="38400" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MinCount_summary_KZ-withimm" sheetId="2" r:id="rId1"/>
@@ -1009,7 +1009,7 @@
   <dimension ref="A1:Y28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V34" sqref="V34"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1640,7 +1640,7 @@
         <v>48.8</v>
       </c>
       <c r="T18">
-        <f>(AVERAGE(J18:K18)/(Q18-R18))-S18</f>
+        <f t="shared" ref="T18:T28" si="6">(AVERAGE(J18:K18)/(Q18-R18))-S18</f>
         <v>6.6545454545454561</v>
       </c>
       <c r="U18">
@@ -1713,11 +1713,11 @@
         <v>0.64</v>
       </c>
       <c r="O19">
-        <f t="shared" ref="O19:O28" si="6">AVERAGE(J19:K19)</f>
+        <f t="shared" ref="O19:O28" si="7">AVERAGE(J19:K19)</f>
         <v>37.799999999999997</v>
       </c>
       <c r="P19">
-        <f t="shared" ref="P19:P28" si="7">AVERAGE(H19:I19)</f>
+        <f t="shared" ref="P19:P28" si="8">AVERAGE(H19:I19)</f>
         <v>7.2000000000000011</v>
       </c>
       <c r="Q19">
@@ -1731,7 +1731,7 @@
         <v>37.799999999999997</v>
       </c>
       <c r="T19">
-        <f>(AVERAGE(J19:K19)/(Q19-R19))-S19</f>
+        <f t="shared" si="6"/>
         <v>3.7384615384615358</v>
       </c>
       <c r="U19">
@@ -1739,7 +1739,7 @@
         <v>7.2000000000000011</v>
       </c>
       <c r="V19">
-        <f t="shared" ref="V19:V28" si="8">(AVERAGE(H19:I19)/(Q19-R19))-U19</f>
+        <f t="shared" ref="V19:V28" si="9">(AVERAGE(H19:I19)/(Q19-R19))-U19</f>
         <v>0.71208791208791222</v>
       </c>
       <c r="W19" s="2" t="s">
@@ -1804,11 +1804,11 @@
         <v>0.64</v>
       </c>
       <c r="O20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>30.8</v>
       </c>
       <c r="P20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5.2</v>
       </c>
       <c r="Q20">
@@ -1822,7 +1822,7 @@
         <v>30.8</v>
       </c>
       <c r="T20">
-        <f>(AVERAGE(J20:K20)/(Q20-R20))-S20</f>
+        <f t="shared" si="6"/>
         <v>3.046153846153846</v>
       </c>
       <c r="U20">
@@ -1830,7 +1830,7 @@
         <v>5.2</v>
       </c>
       <c r="V20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.51428571428571423</v>
       </c>
       <c r="W20" s="2" t="s">
@@ -1884,7 +1884,7 @@
         <v>32</v>
       </c>
       <c r="P21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="Q21">
@@ -1898,7 +1898,7 @@
         <v>32</v>
       </c>
       <c r="T21">
-        <f>(AVERAGE(J21:K21)/(Q21-R21))-S21</f>
+        <f t="shared" si="6"/>
         <v>3.1648351648351607</v>
       </c>
       <c r="U21">
@@ -1906,7 +1906,7 @@
         <v>6</v>
       </c>
       <c r="V21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.59340659340659307</v>
       </c>
       <c r="W21" t="s">
@@ -1918,22 +1918,22 @@
         <v>2015</v>
       </c>
       <c r="E22">
-        <f t="shared" ref="E22:E28" si="9">J22+H22</f>
+        <f t="shared" ref="E22:E28" si="10">J22+H22</f>
         <v>41</v>
       </c>
       <c r="F22">
-        <f t="shared" ref="F22:F28" si="10">K22+I22</f>
+        <f t="shared" ref="F22:F28" si="11">K22+I22</f>
         <v>41</v>
       </c>
       <c r="G22" s="1">
         <v>6</v>
       </c>
       <c r="H22">
-        <f t="shared" ref="H22:I28" si="11">G22</f>
+        <f t="shared" ref="H22:I28" si="12">G22</f>
         <v>6</v>
       </c>
       <c r="I22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="J22">
@@ -1946,18 +1946,18 @@
         <v>25</v>
       </c>
       <c r="M22">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N22">
         <f>AVERAGE(L22:M22)/AVERAGE(J22:K22)</f>
-        <v>0.74285714285714288</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="O22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>35</v>
       </c>
       <c r="P22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="Q22">
@@ -1967,19 +1967,19 @@
         <v>0.09</v>
       </c>
       <c r="S22">
-        <f t="shared" ref="S22:S28" si="12">AVERAGE(J22:K22)/Q22</f>
+        <f t="shared" ref="S22:S28" si="13">AVERAGE(J22:K22)/Q22</f>
         <v>35</v>
       </c>
       <c r="T22">
-        <f>(AVERAGE(J22:K22)/(Q22-R22))-S22</f>
+        <f t="shared" si="6"/>
         <v>3.4615384615384599</v>
       </c>
       <c r="U22">
-        <f t="shared" ref="U22:U28" si="13">AVERAGE(H22:I22)/Q22</f>
+        <f t="shared" ref="U22:U28" si="14">AVERAGE(H22:I22)/Q22</f>
         <v>6</v>
       </c>
       <c r="V22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.59340659340659307</v>
       </c>
       <c r="W22" t="s">
@@ -1991,22 +1991,22 @@
         <v>2016</v>
       </c>
       <c r="E23">
-        <f t="shared" si="9"/>
-        <v>54</v>
-      </c>
-      <c r="F23">
         <f t="shared" si="10"/>
         <v>54</v>
       </c>
+      <c r="F23">
+        <f t="shared" si="11"/>
+        <v>54</v>
+      </c>
       <c r="G23" s="1">
         <v>9</v>
       </c>
       <c r="H23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="I23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="J23">
@@ -2019,18 +2019,18 @@
         <v>29</v>
       </c>
       <c r="M23">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N23">
-        <f t="shared" ref="N23:N28" si="14">AVERAGE(L23:M23)/AVERAGE(J23:K23)</f>
-        <v>0.65555555555555556</v>
+        <f t="shared" ref="N23:N28" si="15">AVERAGE(L23:M23)/AVERAGE(J23:K23)</f>
+        <v>0.64444444444444449</v>
       </c>
       <c r="O23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>45</v>
       </c>
       <c r="P23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="Q23">
@@ -2040,19 +2040,19 @@
         <v>0.09</v>
       </c>
       <c r="S23">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>45</v>
       </c>
       <c r="T23">
-        <f>(AVERAGE(J23:K23)/(Q23-R23))-S23</f>
+        <f t="shared" si="6"/>
         <v>4.4505494505494454</v>
       </c>
       <c r="U23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>9</v>
       </c>
       <c r="V23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.8901098901098905</v>
       </c>
       <c r="W23" t="s">
@@ -2064,22 +2064,22 @@
         <v>2017</v>
       </c>
       <c r="E24">
-        <f t="shared" si="9"/>
-        <v>60</v>
-      </c>
-      <c r="F24">
         <f t="shared" si="10"/>
         <v>60</v>
       </c>
+      <c r="F24">
+        <f t="shared" si="11"/>
+        <v>60</v>
+      </c>
       <c r="G24" s="1">
         <v>12</v>
       </c>
       <c r="H24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
       <c r="I24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12</v>
       </c>
       <c r="J24">
@@ -2092,18 +2092,18 @@
         <v>31</v>
       </c>
       <c r="M24">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="N24">
-        <f t="shared" si="14"/>
-        <v>0.58333333333333337</v>
+        <f t="shared" si="15"/>
+        <v>0.64583333333333337</v>
       </c>
       <c r="O24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
       <c r="P24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="Q24">
@@ -2113,19 +2113,19 @@
         <v>0.09</v>
       </c>
       <c r="S24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>48</v>
       </c>
       <c r="T24">
-        <f>(AVERAGE(J24:K24)/(Q24-R24))-S24</f>
+        <f t="shared" si="6"/>
         <v>4.7472527472527446</v>
       </c>
       <c r="U24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>12</v>
       </c>
       <c r="V24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.1868131868131861</v>
       </c>
       <c r="W24" t="s">
@@ -2137,13 +2137,13 @@
         <v>2018</v>
       </c>
       <c r="E25">
-        <f t="shared" si="9"/>
-        <v>66</v>
-      </c>
-      <c r="F25">
         <f t="shared" si="10"/>
         <v>66</v>
       </c>
+      <c r="F25">
+        <f t="shared" si="11"/>
+        <v>66</v>
+      </c>
       <c r="G25" s="1">
         <v>12</v>
       </c>
@@ -2163,18 +2163,18 @@
         <v>27</v>
       </c>
       <c r="M25">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="N25">
-        <f t="shared" si="14"/>
-        <v>0.57547169811320753</v>
+        <f t="shared" si="15"/>
+        <v>0.50943396226415094</v>
       </c>
       <c r="O25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>53</v>
       </c>
       <c r="P25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="Q25">
@@ -2184,19 +2184,19 @@
         <v>0.09</v>
       </c>
       <c r="S25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>53</v>
       </c>
       <c r="T25">
-        <f>(AVERAGE(J25:K25)/(Q25-R25))-S25</f>
+        <f t="shared" si="6"/>
         <v>5.2417582417582409</v>
       </c>
       <c r="U25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>13</v>
       </c>
       <c r="V25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.2857142857142847</v>
       </c>
       <c r="W25" t="s">
@@ -2208,22 +2208,22 @@
         <v>2019</v>
       </c>
       <c r="E26">
-        <f t="shared" si="9"/>
-        <v>81</v>
-      </c>
-      <c r="F26">
         <f t="shared" si="10"/>
         <v>81</v>
       </c>
+      <c r="F26">
+        <f t="shared" si="11"/>
+        <v>81</v>
+      </c>
       <c r="G26" s="1">
         <v>11</v>
       </c>
       <c r="H26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="I26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="J26">
@@ -2236,18 +2236,18 @@
         <v>39</v>
       </c>
       <c r="M26">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="N26">
-        <f t="shared" si="14"/>
-        <v>0.51428571428571423</v>
+        <f t="shared" si="15"/>
+        <v>0.55714285714285716</v>
       </c>
       <c r="O26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>70</v>
       </c>
       <c r="P26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="Q26">
@@ -2257,19 +2257,19 @@
         <v>0.09</v>
       </c>
       <c r="S26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>70</v>
       </c>
       <c r="T26">
-        <f>(AVERAGE(J26:K26)/(Q26-R26))-S26</f>
+        <f t="shared" si="6"/>
         <v>6.9230769230769198</v>
       </c>
       <c r="U26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>11</v>
       </c>
       <c r="V26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.0879120879120876</v>
       </c>
       <c r="W26" t="s">
@@ -2281,22 +2281,22 @@
         <v>2020</v>
       </c>
       <c r="E27">
-        <f t="shared" si="9"/>
-        <v>84</v>
-      </c>
-      <c r="F27">
         <f t="shared" si="10"/>
         <v>84</v>
       </c>
+      <c r="F27">
+        <f t="shared" si="11"/>
+        <v>84</v>
+      </c>
       <c r="G27" s="1">
         <v>14</v>
       </c>
       <c r="H27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>14</v>
       </c>
       <c r="I27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>14</v>
       </c>
       <c r="J27">
@@ -2309,18 +2309,18 @@
         <v>30</v>
       </c>
       <c r="M27">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N27">
-        <f t="shared" si="14"/>
-        <v>0.42142857142857143</v>
+        <f t="shared" si="15"/>
+        <v>0.42857142857142855</v>
       </c>
       <c r="O27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>70</v>
       </c>
       <c r="P27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="Q27">
@@ -2330,19 +2330,19 @@
         <v>0.09</v>
       </c>
       <c r="S27">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>70</v>
       </c>
       <c r="T27">
-        <f>(AVERAGE(J27:K27)/(Q27-R27))-S27</f>
+        <f t="shared" si="6"/>
         <v>6.9230769230769198</v>
       </c>
       <c r="U27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="V27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.3846153846153832</v>
       </c>
       <c r="W27" t="s">
@@ -2354,22 +2354,22 @@
         <v>2021</v>
       </c>
       <c r="E28">
-        <f t="shared" si="9"/>
-        <v>101</v>
-      </c>
-      <c r="F28">
         <f t="shared" si="10"/>
         <v>101</v>
       </c>
+      <c r="F28">
+        <f t="shared" si="11"/>
+        <v>101</v>
+      </c>
       <c r="G28" s="1">
         <v>14</v>
       </c>
       <c r="H28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>14</v>
       </c>
       <c r="I28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>14</v>
       </c>
       <c r="J28">
@@ -2382,18 +2382,18 @@
         <v>38</v>
       </c>
       <c r="M28">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N28">
-        <f t="shared" si="14"/>
-        <v>0.43103448275862066</v>
+        <f t="shared" si="15"/>
+        <v>0.43678160919540232</v>
       </c>
       <c r="O28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>87</v>
       </c>
       <c r="P28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>14</v>
       </c>
       <c r="Q28">
@@ -2403,19 +2403,19 @@
         <v>0.09</v>
       </c>
       <c r="S28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>87</v>
       </c>
       <c r="T28">
-        <f>(AVERAGE(J28:K28)/(Q28-R28))-S28</f>
+        <f t="shared" si="6"/>
         <v>8.6043956043956058</v>
       </c>
       <c r="U28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="V28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1.3846153846153832</v>
       </c>
       <c r="W28" t="s">

</xml_diff>

<commit_message>
increase plot resolution upon acceptance, double check all files/analysis
</commit_message>
<xml_diff>
--- a/data/KZ/Count_summary_KZ.xlsx
+++ b/data/KZ/Count_summary_KZ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clayton.lamb/Google Drive/Documents/University/PDF/PDF Analyses/KZdemography/KZ_QT_IPM/data/KZ/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clayton.lamb/Dropbox/Documents/University/PDF/PDF Analyses/KZdemography/KZ_QT_IPM/data/KZ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A33053-75A3-834C-92C5-258BC28A478F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5CE2D5-D18E-9F44-AEAD-3028D852D025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40800" yWindow="500" windowWidth="38400" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MinCount_summary_KZ-withimm" sheetId="2" r:id="rId1"/>
@@ -1009,7 +1009,7 @@
   <dimension ref="A1:Y28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2095,7 +2095,7 @@
         <v>31</v>
       </c>
       <c r="N24">
-        <f t="shared" si="15"/>
+        <f>AVERAGE(L24:M24)/AVERAGE(J24:K24)</f>
         <v>0.64583333333333337</v>
       </c>
       <c r="O24">

</xml_diff>